<commit_message>
update log for single mode
</commit_message>
<xml_diff>
--- a/template/Tier1.xlsx
+++ b/template/Tier1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangyaoshen\go\src\github.com\liserjrqlxue\anno2xlsx\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E9B19A-E0A1-484C-B21B-6662C129A5BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA70FA4-7666-49B5-8DE7-5A9F00C30301}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="0" windowWidth="28800" windowHeight="11175" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Tier1" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tier1!$A$1:$EG$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tier1!$A$1:$EH$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
   <si>
     <t>#Chr</t>
   </si>
@@ -437,6 +437,10 @@
   </si>
   <si>
     <t>表型分值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tier</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -501,7 +505,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -509,6 +513,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -848,19 +853,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CFD027B-67B3-43CF-9934-C284ECAEF97B}">
-  <dimension ref="A1:EG1"/>
+  <dimension ref="A1:EH1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="E1:F1048576"/>
+      <selection activeCell="EH1" sqref="CC1:EH1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="6" width="8.796875" hidden="1" customWidth="1"/>
     <col min="81" max="137" width="8.796875" hidden="1" customWidth="1"/>
+    <col min="138" max="138" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:137" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:138" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1272,10 +1278,14 @@
       <c r="EG1" s="4" t="s">
         <v>131</v>
       </c>
+      <c r="EH1" s="5" t="s">
+        <v>137</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:EG1" xr:uid="{44F15860-124D-46CE-B2E3-AA9BDD3F4AE8}"/>
+  <autoFilter ref="A1:EH1" xr:uid="{EF1EE19E-9769-4CC5-A620-39882ECD3329}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CRLF to LF, add 核型预测 to quality
</commit_message>
<xml_diff>
--- a/template/Tier1.xlsx
+++ b/template/Tier1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangyaoshen\go\src\github.com\liserjrqlxue\anno2xlsx\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FEB88D7-9F20-4B18-8F20-BC12667E15F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E89C1B5-BCDE-49B6-A867-5831121A1B3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="0" windowWidth="28800" windowHeight="11175" tabRatio="534" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
   <si>
     <t>#Chr</t>
   </si>
@@ -470,13 +470,17 @@
   </si>
   <si>
     <t>bam文件路径</t>
+  </si>
+  <si>
+    <t>核型预测</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Verdana"/>
@@ -497,6 +501,12 @@
       <color theme="1"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="4">
@@ -533,7 +543,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -544,6 +554,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1325,15 +1338,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5713C2-1176-4A65-9BEF-889DD5EFF094}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.09765625" customWidth="1"/>
+    <col min="1" max="1" width="26.296875" customWidth="1"/>
     <col min="2" max="2" width="25.09765625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1382,8 +1395,14 @@
         <v>146</v>
       </c>
     </row>
+    <row r="10" spans="1:1" ht="17.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
merge tier2 file as sheet to tier1 file
</commit_message>
<xml_diff>
--- a/template/Tier1.xlsx
+++ b/template/Tier1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangyaoshen\go\src\github.com\liserjrqlxue\anno2xlsx\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E89C1B5-BCDE-49B6-A867-5831121A1B3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB312D04-B820-485C-8BFA-3CE0AA78F7B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="0" windowWidth="28800" windowHeight="11175" tabRatio="534" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="filter_variants" sheetId="4" r:id="rId1"/>
-    <sheet name="quality" sheetId="5" r:id="rId2"/>
+    <sheet name="附表" sheetId="6" r:id="rId2"/>
+    <sheet name="quality" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">filter_variants!$A$1:$EH$1</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="148">
   <si>
     <t>#Chr</t>
   </si>
@@ -898,17 +899,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CFD027B-67B3-43CF-9934-C284ECAEF97B}">
   <dimension ref="A1:EH1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView topLeftCell="DG1" workbookViewId="0">
+      <selection sqref="A1:EH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="4" width="8.796875" style="4"/>
-    <col min="5" max="6" width="8.796875" style="4" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="8.796875" style="4" customWidth="1"/>
     <col min="7" max="80" width="8.796875" style="4"/>
-    <col min="81" max="137" width="8.796875" style="4" hidden="1" customWidth="1"/>
-    <col min="138" max="138" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="81" max="138" width="8.796875" style="4" customWidth="1"/>
     <col min="139" max="16384" width="8.796875" style="4"/>
   </cols>
   <sheetData>
@@ -1337,10 +1337,443 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4924BC3-C42A-46AB-9CF7-08322CC791CE}">
+  <dimension ref="A1:EH1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q20:Q21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:138" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AT1" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="BY1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="CC1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="CD1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="CE1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="CF1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="CG1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="CH1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="CI1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="CJ1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="CK1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="CL1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="CM1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="CN1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="CO1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="CP1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="CQ1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="CR1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="CS1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="CT1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="CU1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CV1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="CW1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="CX1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="CY1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="CZ1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="DA1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="DB1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="DC1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="DD1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="DE1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="DF1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="DG1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="DH1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="DI1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="DJ1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="DK1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="DL1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="DM1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="DN1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="DO1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="DP1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="DQ1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="DR1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="DS1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="DT1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="DU1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="DV1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="DW1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="DX1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="DY1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="DZ1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="EA1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="EB1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="EC1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="ED1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="EE1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="EF1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="EG1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="EH1" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5713C2-1176-4A65-9BEF-889DD5EFF094}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add exon_cnv and 20X coverage to template
</commit_message>
<xml_diff>
--- a/template/Tier1.xlsx
+++ b/template/Tier1.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangyaoshen\go\src\github.com\liserjrqlxue\anno2xlsx\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A4DFA5-7E4E-422B-9513-F82FF2965522}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5973060D-6722-4FBF-B157-AB7BCEE6B248}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="0" windowWidth="28800" windowHeight="11175" tabRatio="534" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="filter_variants" sheetId="4" r:id="rId1"/>
     <sheet name="附表" sheetId="6" r:id="rId2"/>
-    <sheet name="large_cnv" sheetId="7" r:id="rId3"/>
-    <sheet name="quality" sheetId="5" r:id="rId4"/>
+    <sheet name="exon_cnv" sheetId="8" r:id="rId3"/>
+    <sheet name="large_cnv" sheetId="7" r:id="rId4"/>
+    <sheet name="quality" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">filter_variants!$A$1:$EH$1</definedName>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="192">
   <si>
     <t>#Chr</t>
   </si>
@@ -551,13 +552,96 @@
   </si>
   <si>
     <t>Omim Gene</t>
+  </si>
+  <si>
+    <t>start.p</t>
+  </si>
+  <si>
+    <t>end.p</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>nexons</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>chromosome</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>BF</t>
+  </si>
+  <si>
+    <t>reads.expected</t>
+  </si>
+  <si>
+    <t>reads.observed</t>
+  </si>
+  <si>
+    <t>reads.ratio</t>
+  </si>
+  <si>
+    <t>Conrad.hg19</t>
+  </si>
+  <si>
+    <t>exons.hg19</t>
+  </si>
+  <si>
+    <t>GeneSymbol</t>
+  </si>
+  <si>
+    <t>OMIM_exon</t>
+  </si>
+  <si>
+    <t>OMIM_chr_start_end</t>
+  </si>
+  <si>
+    <t>CNV_annot</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>目标区平均深度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;20X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>位点所占比例</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Verdana"/>
@@ -588,6 +672,13 @@
     <font>
       <sz val="12"/>
       <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="4">
@@ -627,7 +718,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -641,6 +732,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -985,7 +1078,7 @@
   <dimension ref="A1:EH1"/>
   <sheetViews>
     <sheetView topLeftCell="DG1" workbookViewId="0">
-      <selection sqref="A1:EH1"/>
+      <selection sqref="A1:AL1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1426,7 +1519,7 @@
   <dimension ref="A1:EH1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection sqref="A1:AL1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1855,10 +1948,133 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C065F851-54F3-4238-B766-AF985788DB58}">
+  <dimension ref="A1:AI1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:AI1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="U1" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="V1" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="W1" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="X1" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="Y1" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z1" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA1" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB1" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="AC1" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="AD1" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AE1" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="AF1" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AG1" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="AH1" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="AI1" s="9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4463254D-0A12-497B-8E69-B39F2A77C8F8}">
   <dimension ref="A1:AL1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:AL1"/>
     </sheetView>
   </sheetViews>
@@ -1987,12 +2203,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5713C2-1176-4A65-9BEF-889DD5EFF094}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2036,18 +2252,23 @@
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>145</v>
+    <row r="8" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="17.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+    <row r="11" spans="1:1" ht="17.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>147</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change large cnv column and skip gene no in db
</commit_message>
<xml_diff>
--- a/template/Tier1.xlsx
+++ b/template/Tier1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangyaoshen\go\src\github.com\liserjrqlxue\anno2xlsx\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5973060D-6722-4FBF-B157-AB7BCEE6B248}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA9B559-2AE6-44E5-B664-E9D47CCE5E51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="28800" windowHeight="11175" tabRatio="534" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="28800" windowHeight="11175" tabRatio="534" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="filter_variants" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="193">
   <si>
     <t>#Chr</t>
   </si>
@@ -634,6 +634,10 @@
       </rPr>
       <t>位点所占比例</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OMIM_Phenotype_ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1951,7 +1955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C065F851-54F3-4238-B766-AF985788DB58}">
   <dimension ref="A1:AI1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:AI1"/>
     </sheetView>
   </sheetViews>
@@ -2074,11 +2078,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4463254D-0A12-497B-8E69-B39F2A77C8F8}">
   <dimension ref="A1:AL1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:AL1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AB1" sqref="AB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="12" max="12" width="0" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
@@ -2163,25 +2171,25 @@
         <v>172</v>
       </c>
       <c r="AB1" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC1" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="AC1" s="7" t="s">
-        <v>102</v>
-      </c>
       <c r="AD1" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="AE1" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="AE1" s="7" t="s">
+      <c r="AF1" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="AF1" s="7" t="s">
+      <c r="AG1" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="AG1" s="7" t="s">
+      <c r="AH1" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="AH1" s="7" t="s">
-        <v>108</v>
       </c>
       <c r="AI1" s="7" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
烈性突变，HGMDorClinvar由兰变黄，需要展示 GERP++_RS_pred顺序移动到PhyloP Placental Mammals Pred后 注释表中加入四列新内容：Lab-CH，Onset age，death age，imprinted gene
</commit_message>
<xml_diff>
--- a/template/Tier1.xlsx
+++ b/template/Tier1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangyaoshen\go\src\github.com\liserjrqlxue\anno2xlsx\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA9B559-2AE6-44E5-B664-E9D47CCE5E51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A15E9C-E7D7-4723-BFE5-D7FEC8CE519D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="28800" windowHeight="11175" tabRatio="534" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="28800" windowHeight="11175" tabRatio="534" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="filter_variants" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="198">
   <si>
     <t>#Chr</t>
   </si>
@@ -639,6 +639,22 @@
   <si>
     <t>OMIM_Phenotype_ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HGMDorClinvar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lab-CH</t>
+  </si>
+  <si>
+    <t>Onset age</t>
+  </si>
+  <si>
+    <t>death age</t>
+  </si>
+  <si>
+    <t>imprinted gene</t>
   </si>
 </sst>
 </file>
@@ -1081,16 +1097,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CFD027B-67B3-43CF-9934-C284ECAEF97B}">
   <dimension ref="A1:EH1"/>
   <sheetViews>
-    <sheetView topLeftCell="DG1" workbookViewId="0">
-      <selection sqref="A1:AL1"/>
+    <sheetView topLeftCell="BQ1" workbookViewId="0">
+      <selection activeCell="CE1" sqref="CE1:EH1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="4" width="8.796875" style="4"/>
-    <col min="5" max="6" width="8.796875" style="4" customWidth="1"/>
-    <col min="7" max="80" width="8.796875" style="4"/>
-    <col min="81" max="138" width="8.796875" style="4" customWidth="1"/>
+    <col min="5" max="6" width="8.796875" style="4" hidden="1" customWidth="1"/>
+    <col min="7" max="82" width="8.796875" style="4"/>
+    <col min="83" max="138" width="8.796875" style="4" hidden="1" customWidth="1"/>
     <col min="139" max="16384" width="8.796875" style="4"/>
   </cols>
   <sheetData>
@@ -1207,22 +1223,22 @@
         <v>66</v>
       </c>
       <c r="AL1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="AR1" s="1" t="s">
         <v>83</v>
@@ -1234,265 +1250,265 @@
         <v>135</v>
       </c>
       <c r="AU1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AV1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="CB1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CC1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CD1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="CC1" s="2" t="s">
+      <c r="CE1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="CD1" s="2" t="s">
+      <c r="CF1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="CE1" s="2" t="s">
+      <c r="CG1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="CF1" s="2" t="s">
+      <c r="CH1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="CG1" s="2" t="s">
+      <c r="CI1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="CH1" s="2" t="s">
+      <c r="CJ1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="CI1" s="2" t="s">
+      <c r="CK1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="CJ1" s="2" t="s">
+      <c r="CL1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="CK1" s="2" t="s">
+      <c r="CM1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="CL1" s="2" t="s">
+      <c r="CN1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="CM1" s="2" t="s">
+      <c r="CO1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="CN1" s="2" t="s">
+      <c r="CP1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="CO1" s="2" t="s">
+      <c r="CQ1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="CP1" s="2" t="s">
+      <c r="CR1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="CQ1" s="2" t="s">
+      <c r="CS1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="CR1" s="2" t="s">
+      <c r="CT1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="CS1" s="2" t="s">
+      <c r="CU1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="CT1" s="2" t="s">
+      <c r="CV1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="CU1" s="2" t="s">
+      <c r="CW1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="CV1" s="2" t="s">
+      <c r="CX1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="CW1" s="2" t="s">
+      <c r="CY1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="CX1" s="2" t="s">
+      <c r="CZ1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="CY1" s="2" t="s">
+      <c r="DA1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="CZ1" s="2" t="s">
+      <c r="DB1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="DA1" s="2" t="s">
+      <c r="DC1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="DB1" s="2" t="s">
+      <c r="DD1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="DC1" s="2" t="s">
+      <c r="DE1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="DD1" s="2" t="s">
+      <c r="DF1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="DE1" s="2" t="s">
+      <c r="DG1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="DF1" s="2" t="s">
+      <c r="DH1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="DG1" s="2" t="s">
+      <c r="DI1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="DH1" s="2" t="s">
+      <c r="DJ1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="DI1" s="2" t="s">
+      <c r="DK1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="DJ1" s="2" t="s">
+      <c r="DL1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="DK1" s="2" t="s">
+      <c r="DM1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="DL1" s="2" t="s">
+      <c r="DN1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="DM1" s="2" t="s">
+      <c r="DO1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="DN1" s="2" t="s">
+      <c r="DP1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="DO1" s="2" t="s">
+      <c r="DQ1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="DP1" s="2" t="s">
+      <c r="DR1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="DQ1" s="2" t="s">
+      <c r="DS1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="DR1" s="2" t="s">
+      <c r="DT1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="DS1" s="2" t="s">
+      <c r="DU1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="DT1" s="2" t="s">
+      <c r="DV1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="DU1" s="2" t="s">
+      <c r="DW1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="DV1" s="2" t="s">
+      <c r="DX1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="DW1" s="2" t="s">
+      <c r="DY1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="DX1" s="2" t="s">
+      <c r="DZ1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="DY1" s="2" t="s">
+      <c r="EA1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="DZ1" s="2" t="s">
+      <c r="EB1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="EA1" s="2" t="s">
+      <c r="EC1" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="EB1" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="EC1" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="ED1" s="2" t="s">
         <v>125</v>
@@ -1520,15 +1536,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4924BC3-C42A-46AB-9CF7-08322CC791CE}">
-  <dimension ref="A1:EH1"/>
+  <dimension ref="A1:EL1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:AL1"/>
+    <sheetView tabSelected="1" topLeftCell="BC1" workbookViewId="0">
+      <selection activeCell="BG1" sqref="BG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="87" max="142" width="8.796875" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:138" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:142" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1641,22 +1661,22 @@
         <v>66</v>
       </c>
       <c r="AL1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="AR1" s="1" t="s">
         <v>83</v>
@@ -1668,279 +1688,291 @@
         <v>135</v>
       </c>
       <c r="AU1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="AV1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="BR1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="CB1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="CC1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="CD1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CE1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="CF1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CG1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CH1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="CC1" s="2" t="s">
+      <c r="CI1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="CD1" s="2" t="s">
+      <c r="CJ1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="CE1" s="2" t="s">
+      <c r="CK1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="CF1" s="2" t="s">
+      <c r="CL1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="CG1" s="2" t="s">
+      <c r="CM1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="CH1" s="2" t="s">
+      <c r="CN1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="CI1" s="2" t="s">
+      <c r="CO1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="CJ1" s="2" t="s">
+      <c r="CP1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="CK1" s="2" t="s">
+      <c r="CQ1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="CL1" s="2" t="s">
+      <c r="CR1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="CM1" s="2" t="s">
+      <c r="CS1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="CN1" s="2" t="s">
+      <c r="CT1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="CO1" s="2" t="s">
+      <c r="CU1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="CP1" s="2" t="s">
+      <c r="CV1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="CQ1" s="2" t="s">
+      <c r="CW1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="CR1" s="2" t="s">
+      <c r="CX1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="CS1" s="2" t="s">
+      <c r="CY1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="CT1" s="2" t="s">
+      <c r="CZ1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="CU1" s="2" t="s">
+      <c r="DA1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="CV1" s="2" t="s">
+      <c r="DB1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="CW1" s="2" t="s">
+      <c r="DC1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="CX1" s="2" t="s">
+      <c r="DD1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="CY1" s="2" t="s">
+      <c r="DE1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="CZ1" s="2" t="s">
+      <c r="DF1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="DA1" s="2" t="s">
+      <c r="DG1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="DB1" s="2" t="s">
+      <c r="DH1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="DC1" s="2" t="s">
+      <c r="DI1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="DD1" s="2" t="s">
+      <c r="DJ1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="DE1" s="2" t="s">
+      <c r="DK1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="DF1" s="2" t="s">
+      <c r="DL1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="DG1" s="2" t="s">
+      <c r="DM1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="DH1" s="2" t="s">
+      <c r="DN1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="DI1" s="2" t="s">
+      <c r="DO1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="DJ1" s="2" t="s">
+      <c r="DP1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="DK1" s="2" t="s">
+      <c r="DQ1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="DL1" s="2" t="s">
+      <c r="DR1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="DM1" s="2" t="s">
+      <c r="DS1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="DN1" s="2" t="s">
+      <c r="DT1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="DO1" s="2" t="s">
+      <c r="DU1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="DP1" s="2" t="s">
+      <c r="DV1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="DQ1" s="2" t="s">
+      <c r="DW1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="DR1" s="2" t="s">
+      <c r="DX1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="DS1" s="2" t="s">
+      <c r="DY1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="DT1" s="2" t="s">
+      <c r="DZ1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="DU1" s="2" t="s">
+      <c r="EA1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="DV1" s="2" t="s">
+      <c r="EB1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="DW1" s="2" t="s">
+      <c r="EC1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="DX1" s="2" t="s">
+      <c r="ED1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="DY1" s="2" t="s">
+      <c r="EE1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="DZ1" s="2" t="s">
+      <c r="EF1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="EA1" s="2" t="s">
+      <c r="EG1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="EB1" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="EC1" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="ED1" s="2" t="s">
+      <c r="EH1" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="EE1" s="2" t="s">
+      <c r="EI1" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="EF1" s="2" t="s">
+      <c r="EJ1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="EG1" s="2" t="s">
+      <c r="EK1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="EH1" s="2" t="s">
+      <c r="EL1" s="2" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2078,8 +2110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4463254D-0A12-497B-8E69-B39F2A77C8F8}">
   <dimension ref="A1:AL1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="AB1" sqref="AB1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AD1" sqref="AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2216,7 +2248,7 @@
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
change geneDiseaseDbColumn for title conflict
</commit_message>
<xml_diff>
--- a/template/Tier1.xlsx
+++ b/template/Tier1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangyaoshen\go\src\github.com\liserjrqlxue\anno2xlsx\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3E2FE4-309E-4298-B4D8-72912916F1F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B538EA1D-149B-43E5-A16D-C94A9AA15CE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="0" windowWidth="28800" windowHeight="11175" tabRatio="534" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="198">
   <si>
     <t>#Chr</t>
   </si>
@@ -1985,15 +1985,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C065F851-54F3-4238-B766-AF985788DB58}">
-  <dimension ref="A1:AI1"/>
+  <dimension ref="A1:AH1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1"/>
+      <selection activeCell="Z1" sqref="Z1:Z1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>148</v>
       </c>
@@ -2070,33 +2070,30 @@
         <v>108</v>
       </c>
       <c r="Z1" s="9" t="s">
-        <v>107</v>
+        <v>192</v>
       </c>
       <c r="AA1" s="9" t="s">
-        <v>192</v>
+        <v>103</v>
       </c>
       <c r="AB1" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AC1" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AD1" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE1" s="9" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="AF1" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AG1" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AH1" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI1" s="9" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2108,10 +2105,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4463254D-0A12-497B-8E69-B39F2A77C8F8}">
-  <dimension ref="A1:AL1"/>
+  <dimension ref="A1:AK1"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="AD1" sqref="AD1"/>
+      <selection activeCell="AC1" sqref="AC1:AC1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2120,7 +2117,7 @@
     <col min="14" max="14" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>148</v>
       </c>
@@ -2206,33 +2203,30 @@
         <v>108</v>
       </c>
       <c r="AC1" s="7" t="s">
-        <v>107</v>
+        <v>192</v>
       </c>
       <c r="AD1" s="7" t="s">
-        <v>192</v>
+        <v>103</v>
       </c>
       <c r="AE1" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AF1" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AG1" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AH1" s="7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="AI1" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AJ1" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AK1" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="AL1" s="7" t="s">
         <v>112</v>
       </c>
     </row>

</xml_diff>

<commit_message>
use geneDiseaseDbTitle to control geneDiseaseDb
</commit_message>
<xml_diff>
--- a/template/Tier1.xlsx
+++ b/template/Tier1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangyaoshen\go\src\github.com\liserjrqlxue\anno2xlsx\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B538EA1D-149B-43E5-A16D-C94A9AA15CE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA20D2B9-CB7F-42BC-A537-BEAECB1CFBBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="28800" windowHeight="11175" tabRatio="534" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="28800" windowHeight="11175" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="filter_variants" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="quality" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">filter_variants!$A$1:$EH$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">filter_variants!$A$1:$EL$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -1095,22 +1095,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CFD027B-67B3-43CF-9934-C284ECAEF97B}">
-  <dimension ref="A1:EH1"/>
+  <dimension ref="A1:EL1"/>
   <sheetViews>
-    <sheetView topLeftCell="BQ1" workbookViewId="0">
-      <selection activeCell="CE1" sqref="CE1:EH1048576"/>
+    <sheetView tabSelected="1" topLeftCell="BC1" workbookViewId="0">
+      <selection activeCell="BN1" sqref="BN1:BQ1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="4" width="8.796875" style="4"/>
     <col min="5" max="6" width="8.796875" style="4" hidden="1" customWidth="1"/>
-    <col min="7" max="82" width="8.796875" style="4"/>
-    <col min="83" max="138" width="8.796875" style="4" hidden="1" customWidth="1"/>
-    <col min="139" max="16384" width="8.796875" style="4"/>
+    <col min="7" max="65" width="8.796875" style="4"/>
+    <col min="70" max="86" width="8.796875" style="4"/>
+    <col min="87" max="142" width="8.796875" style="4" hidden="1" customWidth="1"/>
+    <col min="143" max="16384" width="8.796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:138" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:142" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1307,227 +1308,239 @@
         <v>112</v>
       </c>
       <c r="BN1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="BR1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="CB1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="CC1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CD1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CE1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CF1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CG1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="CD1" s="1" t="s">
+      <c r="CH1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="CE1" s="2" t="s">
+      <c r="CI1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="CF1" s="2" t="s">
+      <c r="CJ1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="CG1" s="2" t="s">
+      <c r="CK1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="CH1" s="2" t="s">
+      <c r="CL1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="CI1" s="2" t="s">
+      <c r="CM1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="CJ1" s="2" t="s">
+      <c r="CN1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="CK1" s="2" t="s">
+      <c r="CO1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="CL1" s="2" t="s">
+      <c r="CP1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="CM1" s="2" t="s">
+      <c r="CQ1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="CN1" s="2" t="s">
+      <c r="CR1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="CO1" s="2" t="s">
+      <c r="CS1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="CP1" s="2" t="s">
+      <c r="CT1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="CQ1" s="2" t="s">
+      <c r="CU1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="CR1" s="2" t="s">
+      <c r="CV1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="CS1" s="2" t="s">
+      <c r="CW1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="CT1" s="2" t="s">
+      <c r="CX1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="CU1" s="2" t="s">
+      <c r="CY1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="CV1" s="2" t="s">
+      <c r="CZ1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="CW1" s="2" t="s">
+      <c r="DA1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="CX1" s="2" t="s">
+      <c r="DB1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="CY1" s="2" t="s">
+      <c r="DC1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="CZ1" s="2" t="s">
+      <c r="DD1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="DA1" s="2" t="s">
+      <c r="DE1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="DB1" s="2" t="s">
+      <c r="DF1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="DC1" s="2" t="s">
+      <c r="DG1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="DD1" s="2" t="s">
+      <c r="DH1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="DE1" s="2" t="s">
+      <c r="DI1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="DF1" s="2" t="s">
+      <c r="DJ1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="DG1" s="2" t="s">
+      <c r="DK1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="DH1" s="2" t="s">
+      <c r="DL1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="DI1" s="2" t="s">
+      <c r="DM1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="DJ1" s="2" t="s">
+      <c r="DN1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="DK1" s="2" t="s">
+      <c r="DO1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="DL1" s="2" t="s">
+      <c r="DP1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="DM1" s="2" t="s">
+      <c r="DQ1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="DN1" s="2" t="s">
+      <c r="DR1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="DO1" s="2" t="s">
+      <c r="DS1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="DP1" s="2" t="s">
+      <c r="DT1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="DQ1" s="2" t="s">
+      <c r="DU1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="DR1" s="2" t="s">
+      <c r="DV1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="DS1" s="2" t="s">
+      <c r="DW1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="DT1" s="2" t="s">
+      <c r="DX1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="DU1" s="2" t="s">
+      <c r="DY1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="DV1" s="2" t="s">
+      <c r="DZ1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="DW1" s="2" t="s">
+      <c r="EA1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="DX1" s="2" t="s">
+      <c r="EB1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="DY1" s="2" t="s">
+      <c r="EC1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="DZ1" s="2" t="s">
+      <c r="ED1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="EA1" s="2" t="s">
+      <c r="EE1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="EB1" s="2" t="s">
+      <c r="EF1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="EC1" s="2" t="s">
+      <c r="EG1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="ED1" s="2" t="s">
+      <c r="EH1" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="EE1" s="2" t="s">
+      <c r="EI1" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="EF1" s="2" t="s">
+      <c r="EJ1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="EG1" s="2" t="s">
+      <c r="EK1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="EH1" s="2" t="s">
+      <c r="EL1" s="2" t="s">
         <v>137</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:EH1" xr:uid="{EF1EE19E-9769-4CC5-A620-39882ECD3329}"/>
+  <autoFilter ref="A1:EL1" xr:uid="{EF1EE19E-9769-4CC5-A620-39882ECD3329}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -1539,7 +1552,7 @@
   <dimension ref="A1:EL1"/>
   <sheetViews>
     <sheetView topLeftCell="BC1" workbookViewId="0">
-      <selection activeCell="BG1" sqref="BG1"/>
+      <selection activeCell="BN1" sqref="BN1:BQ1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1743,18 +1756,6 @@
       </c>
       <c r="BM1" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="BO1" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="BQ1" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="BR1" s="1" t="s">
         <v>113</v>
@@ -1987,7 +1988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C065F851-54F3-4238-B766-AF985788DB58}">
   <dimension ref="A1:AH1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="Z1" sqref="Z1:Z1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
change cnv column title
</commit_message>
<xml_diff>
--- a/template/Tier1.xlsx
+++ b/template/Tier1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangyaoshen\go\src\github.com\liserjrqlxue\anno2xlsx\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA20D2B9-CB7F-42BC-A537-BEAECB1CFBBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384F66D6-F070-46A4-8B95-B308F95E4F8A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="28800" windowHeight="11175" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="534" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="filter_variants" sheetId="4" r:id="rId1"/>
@@ -22,12 +22,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">filter_variants!$A$1:$EL$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="199">
   <si>
     <t>#Chr</t>
   </si>
@@ -594,9 +602,6 @@
   </si>
   <si>
     <t>exons.hg19</t>
-  </si>
-  <si>
-    <t>GeneSymbol</t>
   </si>
   <si>
     <t>OMIM_exon</t>
@@ -655,6 +660,14 @@
   </si>
   <si>
     <t>imprinted gene</t>
+  </si>
+  <si>
+    <t>Gene</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OMIM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1097,7 +1110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CFD027B-67B3-43CF-9934-C284ECAEF97B}">
   <dimension ref="A1:EL1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BC1" workbookViewId="0">
+    <sheetView topLeftCell="BC1" workbookViewId="0">
       <selection activeCell="BN1" sqref="BN1:BQ1048576"/>
     </sheetView>
   </sheetViews>
@@ -1308,16 +1321,16 @@
         <v>112</v>
       </c>
       <c r="BN1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="BO1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="BQ1" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="BR1" s="1" t="s">
         <v>113</v>
@@ -1701,7 +1714,7 @@
         <v>135</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AV1" s="1" t="s">
         <v>43</v>
@@ -1989,7 +2002,7 @@
   <dimension ref="A1:AH1"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1:Z1048576"/>
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2047,19 +2060,19 @@
         <v>8</v>
       </c>
       <c r="R1" s="9" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="S1" s="9" t="s">
         <v>158</v>
       </c>
       <c r="T1" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="U1" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="V1" s="9" t="s">
         <v>189</v>
-      </c>
-      <c r="V1" s="9" t="s">
-        <v>190</v>
       </c>
       <c r="W1" s="9" t="s">
         <v>159</v>
@@ -2071,7 +2084,7 @@
         <v>108</v>
       </c>
       <c r="Z1" s="9" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="AA1" s="9" t="s">
         <v>103</v>
@@ -2101,6 +2114,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2108,8 +2122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4463254D-0A12-497B-8E69-B39F2A77C8F8}">
   <dimension ref="A1:AK1"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="AC1" sqref="AC1:AC1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2204,7 +2218,7 @@
         <v>108</v>
       </c>
       <c r="AC1" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AD1" s="7" t="s">
         <v>103</v>
@@ -2289,7 +2303,7 @@
     </row>
     <row r="8" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
change death age to hpo_cn
</commit_message>
<xml_diff>
--- a/template/Tier1.xlsx
+++ b/template/Tier1.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangyaoshen\go\src\github.com\liserjrqlxue\anno2xlsx\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384F66D6-F070-46A4-8B95-B308F95E4F8A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EA0DDA-0150-4C36-ACB3-AF1A6AC7C3B6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="534" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="filter_variants" sheetId="4" r:id="rId1"/>
-    <sheet name="附表" sheetId="6" r:id="rId2"/>
-    <sheet name="exon_cnv" sheetId="8" r:id="rId3"/>
-    <sheet name="large_cnv" sheetId="7" r:id="rId4"/>
-    <sheet name="quality" sheetId="5" r:id="rId5"/>
+    <sheet name="exon_cnv" sheetId="8" r:id="rId2"/>
+    <sheet name="large_cnv" sheetId="7" r:id="rId3"/>
+    <sheet name="quality" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">filter_variants!$A$1:$EL$1</definedName>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="198">
   <si>
     <t>#Chr</t>
   </si>
@@ -646,17 +645,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>HGMDorClinvar</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Lab-CH</t>
   </si>
   <si>
     <t>Onset age</t>
-  </si>
-  <si>
-    <t>death age</t>
   </si>
   <si>
     <t>imprinted gene</t>
@@ -667,6 +659,10 @@
   </si>
   <si>
     <t>OMIM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hpo_cn</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1110,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CFD027B-67B3-43CF-9934-C284ECAEF97B}">
   <dimension ref="A1:EL1"/>
   <sheetViews>
-    <sheetView topLeftCell="BC1" workbookViewId="0">
-      <selection activeCell="BN1" sqref="BN1:BQ1048576"/>
+    <sheetView tabSelected="1" topLeftCell="BG1" workbookViewId="0">
+      <selection activeCell="BP1" sqref="BP1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1321,16 +1317,16 @@
         <v>112</v>
       </c>
       <c r="BN1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="BO1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="BQ1" s="1" t="s">
-        <v>196</v>
       </c>
       <c r="BR1" s="1" t="s">
         <v>113</v>
@@ -1561,443 +1557,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4924BC3-C42A-46AB-9CF7-08322CC791CE}">
-  <dimension ref="A1:EL1"/>
-  <sheetViews>
-    <sheetView topLeftCell="BC1" workbookViewId="0">
-      <selection activeCell="BN1" sqref="BN1:BQ1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="5" max="6" width="0" hidden="1" customWidth="1"/>
-    <col min="87" max="142" width="8.796875" hidden="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:142" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="AT1" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="BE1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="BG1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="BH1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="BI1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="BK1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="BL1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="BM1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="BR1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="BS1" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="BT1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="BU1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="BV1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="BW1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="BX1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="BY1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="BZ1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="CA1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="CB1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="CC1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="CD1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="CE1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="CF1" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="CG1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="CH1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="CI1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="CJ1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="CK1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="CL1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="CM1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="CN1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="CO1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="CP1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="CQ1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="CR1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="CS1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="CT1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="CU1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="CV1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="CW1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="CX1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="CY1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="CZ1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="DA1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DB1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="DC1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="DD1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="DE1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="DF1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="DG1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="DH1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="DI1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="DJ1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="DK1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="DL1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="DM1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="DN1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="DO1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="DP1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="DQ1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="DR1" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="DS1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="DT1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="DU1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="DV1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="DW1" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="DX1" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="DY1" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="DZ1" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="EA1" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="EB1" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="EC1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="ED1" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="EE1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="EF1" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="EG1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="EH1" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="EI1" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="EJ1" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="EK1" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="EL1" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C065F851-54F3-4238-B766-AF985788DB58}">
   <dimension ref="A1:AH1"/>
   <sheetViews>
@@ -2060,7 +1619,7 @@
         <v>8</v>
       </c>
       <c r="R1" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="S1" s="9" t="s">
         <v>158</v>
@@ -2084,7 +1643,7 @@
         <v>108</v>
       </c>
       <c r="Z1" s="9" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AA1" s="9" t="s">
         <v>103</v>
@@ -2118,11 +1677,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4463254D-0A12-497B-8E69-B39F2A77C8F8}">
   <dimension ref="A1:AK1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
@@ -2252,7 +1811,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5713C2-1176-4A65-9BEF-889DD5EFF094}">
   <dimension ref="A1:A11"/>
   <sheetViews>

</xml_diff>

<commit_message>
add HGMD content column for exon cnv
</commit_message>
<xml_diff>
--- a/template/Tier1.xlsx
+++ b/template/Tier1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangyaoshen\go\src\github.com\liserjrqlxue\anno2xlsx\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BABCA94-9666-498E-B82C-D883AB74C520}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFEFB27A-3910-4C26-A2E0-3863BEA18D3B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="534" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="534" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="filter_variants" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="201">
   <si>
     <t>#Chr</t>
   </si>
@@ -966,6 +966,10 @@
   </si>
   <si>
     <t>Primer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HGMD content</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1873,10 +1877,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C065F851-54F3-4238-B766-AF985788DB58}">
-  <dimension ref="A1:AI1"/>
+  <dimension ref="A1:AJ1"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AI1" sqref="AI1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AJ1" sqref="AJ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
@@ -1884,7 +1888,7 @@
     <col min="1" max="16384" width="8.796875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>125</v>
       </c>
@@ -1989,6 +1993,9 @@
       </c>
       <c r="AI1" s="5" t="s">
         <v>199</v>
+      </c>
+      <c r="AJ1" s="5" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2002,7 +2009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4463254D-0A12-497B-8E69-B39F2A77C8F8}">
   <dimension ref="A1:AL1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="AL2" sqref="AL2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
remove quality sheet from template
</commit_message>
<xml_diff>
--- a/template/Tier1.xlsx
+++ b/template/Tier1.xlsx
@@ -5,18 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A\go\src\github.com\liserjrqlxue\anno2xlsx\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangyaoshen\go\src\github.com\liserjrqlxue\anno2xlsx\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D02C640-6AED-4C2E-8C06-04E32BEAA76E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFE0BB1-3CA1-447C-8BE7-C81CD045E42D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1155" yWindow="-120" windowWidth="37365" windowHeight="16440" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="filter_variants" sheetId="4" r:id="rId1"/>
     <sheet name="exon_cnv" sheetId="8" r:id="rId2"/>
     <sheet name="large_cnv" sheetId="7" r:id="rId3"/>
-    <sheet name="quality" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">filter_variants!$A$1:$EM$1</definedName>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="190">
   <si>
     <t>#Chr</t>
   </si>
@@ -735,236 +734,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>样本编号</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>原始数据产出（</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Mb</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>目标区长度（</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>bp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>目标区覆盖度</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>目标区平均深度（</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>X</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>目标区平均深度</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>&gt;4X</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>位点所占比例</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>目标区平均深度</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>&gt;10X</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>位点所占比例</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>目标区平均深度</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>&gt;20X</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>位点所占比例</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>目标区平均深度</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>&gt;30X</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>位点所占比例</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>bam</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>文件路径</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>核型预测</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Primer</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -977,7 +746,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Verdana"/>
@@ -992,12 +761,6 @@
       <sz val="10"/>
       <name val="Verdana"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="微软雅黑"/>
-      <family val="2"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1064,21 +827,20 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1992,10 +1754,10 @@
         <v>110</v>
       </c>
       <c r="AI1" s="5" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="AJ1" s="5" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2135,84 +1897,7 @@
         <v>110</v>
       </c>
       <c r="AL1" s="5" t="s">
-        <v>199</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5713C2-1176-4A65-9BEF-889DD5EFF094}">
-  <dimension ref="A1:A11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="26.296875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="25.09765625" style="5" customWidth="1"/>
-    <col min="3" max="16384" width="8.796875" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
         <v>188</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="17.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>